<commit_message>
Finalização - 03/04 - 17:12
</commit_message>
<xml_diff>
--- a/Banco de Dados/Consumo_cafe.xlsx
+++ b/Banco de Dados/Consumo_cafe.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" autoCompressPictures="0"/>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{ECD9B465-D905-42B6-B2F6-F7B6E276B0DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E5D782E5-7D31-437E-B020-0CCB0A7731A0}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="8_{ECD9B465-D905-42B6-B2F6-F7B6E276B0DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6070EAC0-174F-4A4E-AF3E-6A3EB88403C9}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="966" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="30" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="181029"/>
   <fileRecoveryPr autoRecover="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -19,9 +19,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
@@ -31,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
   <si>
     <t>Paises</t>
   </si>
@@ -51,93 +49,33 @@
     <t>Brazil</t>
   </si>
   <si>
-    <t>21 997</t>
-  </si>
-  <si>
-    <t>22 200</t>
-  </si>
-  <si>
     <t>Indonesia</t>
   </si>
   <si>
-    <t>4 750</t>
-  </si>
-  <si>
-    <t>4 800</t>
-  </si>
-  <si>
     <t>Ethiopia</t>
   </si>
   <si>
-    <t>3 643</t>
-  </si>
-  <si>
-    <t>3 685</t>
-  </si>
-  <si>
     <t>Philippines</t>
   </si>
   <si>
-    <t>3 180</t>
-  </si>
-  <si>
-    <t>3 300</t>
-  </si>
-  <si>
     <t>Viet Nam</t>
   </si>
   <si>
-    <t>2 500</t>
-  </si>
-  <si>
-    <t>2 600</t>
-  </si>
-  <si>
     <t>Mexico</t>
   </si>
   <si>
-    <t>2 400</t>
-  </si>
-  <si>
-    <t>2 450</t>
-  </si>
-  <si>
     <t>Colombia</t>
   </si>
   <si>
-    <t>1 793</t>
-  </si>
-  <si>
-    <t>1 791</t>
-  </si>
-  <si>
     <t>Venezuela</t>
   </si>
   <si>
-    <t>1 600</t>
-  </si>
-  <si>
-    <t>1 550</t>
-  </si>
-  <si>
     <t>India</t>
   </si>
   <si>
-    <t>1 470</t>
-  </si>
-  <si>
-    <t>1 475</t>
-  </si>
-  <si>
     <t>Thailand</t>
   </si>
   <si>
-    <t>1 375</t>
-  </si>
-  <si>
-    <t>1 400</t>
-  </si>
-  <si>
     <t>Guatemala</t>
   </si>
   <si>
@@ -171,76 +109,37 @@
     <t>European Union</t>
   </si>
   <si>
-    <t>40 491</t>
-  </si>
-  <si>
-    <t>41 768</t>
-  </si>
-  <si>
     <t>United States of America</t>
   </si>
   <si>
-    <t>26 112</t>
-  </si>
-  <si>
     <t>Japan</t>
   </si>
   <si>
-    <t>7 750</t>
-  </si>
-  <si>
     <t>Russian Federation</t>
   </si>
   <si>
-    <t>4 324</t>
-  </si>
-  <si>
     <t>Canada</t>
   </si>
   <si>
-    <t>3 829</t>
-  </si>
-  <si>
     <t>Republic of Korea</t>
   </si>
   <si>
-    <t>2 371</t>
-  </si>
-  <si>
     <t>Australia</t>
   </si>
   <si>
-    <t>1 854</t>
-  </si>
-  <si>
     <t>Algeria</t>
   </si>
   <si>
-    <t>1 911</t>
-  </si>
-  <si>
     <t>Turkey</t>
   </si>
   <si>
-    <t>1 376</t>
-  </si>
-  <si>
     <t>Saudi Arabia</t>
   </si>
   <si>
-    <t>1 275</t>
-  </si>
-  <si>
     <t>Ukraine</t>
   </si>
   <si>
-    <t>1 252</t>
-  </si>
-  <si>
     <t>Switzerland</t>
-  </si>
-  <si>
-    <t>1 013</t>
   </si>
   <si>
     <t>Normay</t>
@@ -1397,7 +1296,7 @@
   <dimension ref="A1:E41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C45" sqref="C45"/>
+      <selection activeCell="G40" sqref="G40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1426,11 +1325,11 @@
       <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" t="s">
-        <v>7</v>
+      <c r="B2">
+        <v>21997</v>
+      </c>
+      <c r="C2">
+        <v>22200</v>
       </c>
       <c r="D2">
         <v>22000</v>
@@ -1441,13 +1340,13 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" t="s">
-        <v>10</v>
+        <v>6</v>
+      </c>
+      <c r="B3">
+        <v>4750</v>
+      </c>
+      <c r="C3">
+        <v>4800</v>
       </c>
       <c r="D3">
         <v>4806</v>
@@ -1458,13 +1357,13 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" t="s">
-        <v>13</v>
+        <v>7</v>
+      </c>
+      <c r="B4">
+        <v>3643</v>
+      </c>
+      <c r="C4">
+        <v>3685</v>
       </c>
       <c r="D4">
         <v>3781</v>
@@ -1475,13 +1374,13 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" t="s">
-        <v>16</v>
+        <v>8</v>
+      </c>
+      <c r="B5">
+        <v>3180</v>
+      </c>
+      <c r="C5">
+        <v>3300</v>
       </c>
       <c r="D5">
         <v>3250</v>
@@ -1492,13 +1391,13 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" t="s">
-        <v>19</v>
+        <v>9</v>
+      </c>
+      <c r="B6">
+        <v>2500</v>
+      </c>
+      <c r="C6">
+        <v>2600</v>
       </c>
       <c r="D6">
         <v>2650</v>
@@ -1509,13 +1408,13 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>20</v>
-      </c>
-      <c r="B7" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" t="s">
-        <v>22</v>
+        <v>10</v>
+      </c>
+      <c r="B7">
+        <v>2400</v>
+      </c>
+      <c r="C7">
+        <v>2450</v>
       </c>
       <c r="D7">
         <v>2425</v>
@@ -1526,13 +1425,13 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>23</v>
-      </c>
-      <c r="B8" t="s">
-        <v>24</v>
-      </c>
-      <c r="C8" t="s">
-        <v>25</v>
+        <v>11</v>
+      </c>
+      <c r="B8">
+        <v>1793</v>
+      </c>
+      <c r="C8">
+        <v>1791</v>
       </c>
       <c r="D8">
         <v>2025</v>
@@ -1543,13 +1442,13 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>26</v>
-      </c>
-      <c r="B9" t="s">
-        <v>27</v>
-      </c>
-      <c r="C9" t="s">
-        <v>28</v>
+        <v>12</v>
+      </c>
+      <c r="B9">
+        <v>1600</v>
+      </c>
+      <c r="C9">
+        <v>1550</v>
       </c>
       <c r="D9">
         <v>1275</v>
@@ -1560,13 +1459,13 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>29</v>
-      </c>
-      <c r="B10" t="s">
-        <v>30</v>
-      </c>
-      <c r="C10" t="s">
-        <v>31</v>
+        <v>13</v>
+      </c>
+      <c r="B10">
+        <v>1470</v>
+      </c>
+      <c r="C10">
+        <v>1475</v>
       </c>
       <c r="D10">
         <v>1450</v>
@@ -1577,13 +1476,13 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>32</v>
-      </c>
-      <c r="B11" t="s">
-        <v>33</v>
-      </c>
-      <c r="C11" t="s">
-        <v>34</v>
+        <v>14</v>
+      </c>
+      <c r="B11">
+        <v>1375</v>
+      </c>
+      <c r="C11">
+        <v>1400</v>
       </c>
       <c r="D11">
         <v>1400</v>
@@ -1594,7 +1493,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>35</v>
+        <v>15</v>
       </c>
       <c r="B12">
         <v>395</v>
@@ -1611,7 +1510,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>36</v>
+        <v>16</v>
       </c>
       <c r="B13">
         <v>390</v>
@@ -1628,7 +1527,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
       <c r="B14">
         <v>365</v>
@@ -1645,7 +1544,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>38</v>
+        <v>18</v>
       </c>
       <c r="B15">
         <v>375</v>
@@ -1662,7 +1561,7 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>39</v>
+        <v>19</v>
       </c>
       <c r="B16">
         <v>353</v>
@@ -1679,7 +1578,7 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="B17">
         <v>340</v>
@@ -1696,7 +1595,7 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="B18">
         <v>317</v>
@@ -1713,7 +1612,7 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="B19">
         <v>300</v>
@@ -1730,7 +1629,7 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>43</v>
+        <v>23</v>
       </c>
       <c r="B20">
         <v>250</v>
@@ -1747,7 +1646,7 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>44</v>
+        <v>24</v>
       </c>
       <c r="B21">
         <v>245</v>
@@ -1764,13 +1663,13 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>45</v>
-      </c>
-      <c r="B22" t="s">
-        <v>46</v>
-      </c>
-      <c r="C22" t="s">
-        <v>47</v>
+        <v>25</v>
+      </c>
+      <c r="B22">
+        <v>40491</v>
+      </c>
+      <c r="C22">
+        <v>41768</v>
       </c>
       <c r="D22">
         <v>39758</v>
@@ -1781,10 +1680,10 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>48</v>
-      </c>
-      <c r="B23" t="s">
-        <v>49</v>
+        <v>26</v>
+      </c>
+      <c r="B23">
+        <v>26112</v>
       </c>
       <c r="C23">
         <v>27759</v>
@@ -1798,10 +1697,10 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>50</v>
-      </c>
-      <c r="B24" t="s">
-        <v>51</v>
+        <v>27</v>
+      </c>
+      <c r="B24">
+        <v>7750</v>
       </c>
       <c r="C24">
         <v>7561</v>
@@ -1815,10 +1714,10 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>52</v>
-      </c>
-      <c r="B25" t="s">
-        <v>53</v>
+        <v>28</v>
+      </c>
+      <c r="B25">
+        <v>4324</v>
       </c>
       <c r="C25">
         <v>4691</v>
@@ -1832,10 +1731,10 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>54</v>
-      </c>
-      <c r="B26" t="s">
-        <v>55</v>
+        <v>29</v>
+      </c>
+      <c r="B26">
+        <v>3829</v>
       </c>
       <c r="C26">
         <v>4020</v>
@@ -1849,10 +1748,10 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>56</v>
-      </c>
-      <c r="B27" t="s">
-        <v>57</v>
+        <v>30</v>
+      </c>
+      <c r="B27">
+        <v>2371</v>
       </c>
       <c r="C27">
         <v>2476</v>
@@ -1866,10 +1765,10 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>58</v>
-      </c>
-      <c r="B28" t="s">
-        <v>59</v>
+        <v>31</v>
+      </c>
+      <c r="B28">
+        <v>1854</v>
       </c>
       <c r="C28">
         <v>1961</v>
@@ -1883,10 +1782,10 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>60</v>
-      </c>
-      <c r="B29" t="s">
-        <v>61</v>
+        <v>32</v>
+      </c>
+      <c r="B29">
+        <v>1911</v>
       </c>
       <c r="C29">
         <v>2150</v>
@@ -1900,10 +1799,10 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>62</v>
-      </c>
-      <c r="B30" t="s">
-        <v>63</v>
+        <v>33</v>
+      </c>
+      <c r="B30">
+        <v>1376</v>
       </c>
       <c r="C30">
         <v>1740</v>
@@ -1917,10 +1816,10 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>64</v>
-      </c>
-      <c r="B31" t="s">
-        <v>65</v>
+        <v>34</v>
+      </c>
+      <c r="B31">
+        <v>1275</v>
       </c>
       <c r="C31">
         <v>1266</v>
@@ -1934,10 +1833,10 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>66</v>
-      </c>
-      <c r="B32" t="s">
-        <v>67</v>
+        <v>35</v>
+      </c>
+      <c r="B32">
+        <v>1252</v>
       </c>
       <c r="C32">
         <v>1379</v>
@@ -1951,10 +1850,10 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>68</v>
-      </c>
-      <c r="B33" t="s">
-        <v>69</v>
+        <v>36</v>
+      </c>
+      <c r="B33">
+        <v>1013</v>
       </c>
       <c r="C33">
         <v>1079</v>
@@ -1968,7 +1867,7 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>70</v>
+        <v>37</v>
       </c>
       <c r="B34">
         <v>729</v>
@@ -1985,7 +1884,7 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>71</v>
+        <v>38</v>
       </c>
       <c r="B35">
         <v>740</v>
@@ -2002,7 +1901,7 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>72</v>
+        <v>39</v>
       </c>
       <c r="B36">
         <v>690</v>
@@ -2019,7 +1918,7 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>73</v>
+        <v>40</v>
       </c>
       <c r="B37">
         <v>610</v>
@@ -2036,7 +1935,7 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>74</v>
+        <v>41</v>
       </c>
       <c r="B38">
         <v>638</v>
@@ -2053,7 +1952,7 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>75</v>
+        <v>42</v>
       </c>
       <c r="B39">
         <v>614</v>
@@ -2070,7 +1969,7 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>76</v>
+        <v>43</v>
       </c>
       <c r="B40">
         <v>604</v>
@@ -2087,7 +1986,7 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>77</v>
+        <v>44</v>
       </c>
       <c r="B41">
         <v>605</v>

</xml_diff>